<commit_message>
Carga inicial de cartas, eventos turno inicial, mostrar info en el front, funcionalidad robar carta y mejoras varias
</commit_message>
<xml_diff>
--- a/doc/Material para la memoria/eventos.xlsx
+++ b/doc/Material para la memoria/eventos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROYECTOS\OneCard\doc\Material para la memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9F3A24-1098-4762-96E6-A13D38CEE662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D2D95D-7485-4749-AFF9-FCDE7D6CB77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>COMIENZO JUEGO</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Devolver estado mana</t>
+  </si>
+  <si>
+    <t>(Por defecto inicialmente, si da tiempo se solicitará al usuario para que elija)</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +151,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -164,15 +173,17 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Énfasis3" xfId="2" builtinId="38"/>
@@ -456,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A6:C29"/>
+  <dimension ref="A6:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,59 +480,62 @@
     <col min="3" max="3" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -531,82 +545,83 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="C21" s="2" t="s">
+      <c r="A21" s="2"/>
+      <c r="C21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="2"/>
       <c r="C22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="C23" s="2" t="s">
+      <c r="A23" s="2"/>
+      <c r="C23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="2"/>
       <c r="C24" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="C25" s="2" t="s">
+      <c r="A25" s="2"/>
+      <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="2"/>
       <c r="C26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="C27" s="2" t="s">
+      <c r="A27" s="2"/>
+      <c r="C27" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="A20:A27"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -625,7 +640,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flujo completo de fase inicial. Cartas seleccionables.
</commit_message>
<xml_diff>
--- a/doc/Material para la memoria/eventos.xlsx
+++ b/doc/Material para la memoria/eventos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROYECTOS\OneCard\doc\Material para la memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D2D95D-7485-4749-AFF9-FCDE7D6CB77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B4FE37-886F-43F6-9CA3-0BA6492C1158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>COMIENZO JUEGO</t>
   </si>
@@ -98,6 +98,21 @@
   </si>
   <si>
     <t>(Por defecto inicialmente, si da tiempo se solicitará al usuario para que elija)</t>
+  </si>
+  <si>
+    <t>ROBAR</t>
+  </si>
+  <si>
+    <t>BAJAR_CAMPO</t>
+  </si>
+  <si>
+    <t>BAJAR_NO_CAMPO</t>
+  </si>
+  <si>
+    <t>ATACAR</t>
+  </si>
+  <si>
+    <t>Constantes FASES</t>
   </si>
 </sst>
 </file>
@@ -127,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +172,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -173,17 +194,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Énfasis3" xfId="2" builtinId="38"/>
@@ -467,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A6:D29"/>
+  <dimension ref="A6:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,79 +500,92 @@
     <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="5" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="1" t="s">
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -558,67 +593,79 @@
       </c>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="C21" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="C22" t="s">
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="C22" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
       <c r="C23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="C24" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="C24" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
       <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
       <c r="C26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="C27" s="1" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="C27" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="A20:A27"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B28:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fase de atacar, botón de pasar turno, mostrar informacion de tableros y cartas
</commit_message>
<xml_diff>
--- a/doc/Material para la memoria/eventos.xlsx
+++ b/doc/Material para la memoria/eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROYECTOS\OneCard\doc\Material para la memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B4FE37-886F-43F6-9CA3-0BA6492C1158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C140F43B-B507-4073-A399-D0C9DCF9D6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>COMIENZO JUEGO</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Fases juego (por cada jugador)</t>
   </si>
   <si>
-    <t>Atacar</t>
-  </si>
-  <si>
     <t>Comprobar estado vidas</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>Elegir tripulación</t>
   </si>
   <si>
-    <t>Devolver estado mana</t>
-  </si>
-  <si>
     <t>(Por defecto inicialmente, si da tiempo se solicitará al usuario para que elija)</t>
   </si>
   <si>
@@ -113,6 +107,12 @@
   </si>
   <si>
     <t>Constantes FASES</t>
+  </si>
+  <si>
+    <t>Defender</t>
+  </si>
+  <si>
+    <t>Atacar ** pendiente comprobar maná suficiente</t>
   </si>
 </sst>
 </file>
@@ -142,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +178,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -194,18 +200,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Énfasis3" xfId="2" builtinId="38"/>
@@ -489,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A6:F29"/>
+  <dimension ref="A6:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,168 +511,163 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
+      <c r="F7" t="s">
         <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="5" t="s">
-        <v>15</v>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="6" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="C21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="C22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="C23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="5" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="C24" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="C21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="C22" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="C23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="C24" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="C25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="C26" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="C27" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="A19:A26"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -693,12 +695,12 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -708,12 +710,12 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enrutado front, pantallas ganador y perdedor, funcionalidad atacar, reiniciar partida, y mejoras varias
</commit_message>
<xml_diff>
--- a/doc/Material para la memoria/eventos.xlsx
+++ b/doc/Material para la memoria/eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROYECTOS\OneCard\doc\Material para la memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C140F43B-B507-4073-A399-D0C9DCF9D6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB487ACC-9F86-4726-8871-2CA25270F7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>COMIENZO JUEGO</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Elegir tripulación</t>
   </si>
   <si>
-    <t>(Por defecto inicialmente, si da tiempo se solicitará al usuario para que elija)</t>
-  </si>
-  <si>
     <t>ROBAR</t>
   </si>
   <si>
@@ -112,7 +109,46 @@
     <t>Defender</t>
   </si>
   <si>
-    <t>Atacar ** pendiente comprobar maná suficiente</t>
+    <t>Reiniciar partida</t>
+  </si>
+  <si>
+    <t>Resetear datos de la partida</t>
+  </si>
+  <si>
+    <t>** Unificar ficheros constantes</t>
+  </si>
+  <si>
+    <t>mana = length campos</t>
+  </si>
+  <si>
+    <t>ataque = daño que hace al enemigo</t>
+  </si>
+  <si>
+    <t>energía = coste de mana para atacar</t>
+  </si>
+  <si>
+    <t>Atacar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt; Al hacer click sobre un boton de reiniciar partida (ganador o perdedor) esperar a que el otro jugador también le de</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt;  varios ataques por turno</t>
+  </si>
+  <si>
+    <t>Implementaciones futuras</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt; Por defecto inicialmente, si da tiempo se solicitará al usuario para que elija</t>
+  </si>
+  <si>
+    <t>ESPERANDO_REINICIAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt; Ejecutar la habilidad de la carta mágica</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt; especificar funcionamiento de habilidad de personaje</t>
   </si>
 </sst>
 </file>
@@ -142,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,19 +204,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -200,11 +230,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -212,7 +242,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Énfasis3" xfId="2" builtinId="38"/>
@@ -496,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A6:F28"/>
+  <dimension ref="A6:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,86 +536,99 @@
     <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="106.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
+      <c r="G10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="3" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>12</v>
       </c>
@@ -595,73 +637,107 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="C21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="C21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="C22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="C22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="C23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="C23" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="C24" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="1" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="A19:A26"/>

</xml_diff>

<commit_message>
añadida funcionalidad cartas maginas y mejoras en codigo
</commit_message>
<xml_diff>
--- a/doc/Material para la memoria/eventos.xlsx
+++ b/doc/Material para la memoria/eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROYECTOS\OneCard\doc\Material para la memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB487ACC-9F86-4726-8871-2CA25270F7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8C9C50-4CAC-4CC5-BBFB-550172152AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,48 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>COMIENZO JUEGO</t>
   </si>
@@ -149,6 +180,9 @@
   </si>
   <si>
     <t xml:space="preserve"> =&gt; especificar funcionamiento de habilidad de personaje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  =&gt; Añadir pagina inicial con titulo, selección de tripulacion e informacion general (instrucciones de juego)</t>
   </si>
 </sst>
 </file>
@@ -178,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +248,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -230,12 +270,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -527,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A6:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,10 +582,10 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="4" t="s">
         <v>25</v>
       </c>
@@ -558,6 +599,11 @@
       </c>
       <c r="E7" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -567,10 +613,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="6"/>
       <c r="G10" t="s">
         <v>31</v>
       </c>
@@ -587,6 +633,10 @@
       <c r="C12" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="E12" cm="1">
+        <f t="array" aca="1" ref="E12" ca="1">+C12:E13</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
@@ -594,10 +644,10 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
@@ -629,16 +679,16 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="C20" s="2" t="s">
         <v>14</v>
       </c>
@@ -647,7 +697,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="A21" s="7"/>
       <c r="C21" s="3" t="s">
         <v>4</v>
       </c>
@@ -656,19 +706,19 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="A22" s="7"/>
       <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="7"/>
       <c r="C23" s="3" t="s">
         <v>33</v>
       </c>
@@ -680,28 +730,28 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="C24" s="1" t="s">
+      <c r="A24" s="7"/>
+      <c r="C24" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
+      <c r="A25" s="7"/>
       <c r="C25" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="7"/>
       <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
@@ -709,10 +759,10 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C31" s="2" t="s">

</xml_diff>

<commit_message>
memoria y documentacion varia
</commit_message>
<xml_diff>
--- a/doc/Material para la memoria/eventos.xlsx
+++ b/doc/Material para la memoria/eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROYECTOS\OneCard\doc\Material para la memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8C9C50-4CAC-4CC5-BBFB-550172152AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827BDB72-1FE9-4213-80AD-1D15F92DFC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -212,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,12 +248,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -270,13 +264,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -569,7 +562,7 @@
   <dimension ref="A6:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,10 +575,10 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="4" t="s">
         <v>25</v>
       </c>
@@ -597,12 +590,12 @@
       <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -613,10 +606,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="5"/>
       <c r="G10" t="s">
         <v>31</v>
       </c>
@@ -644,10 +637,10 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
@@ -679,16 +672,16 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="6"/>
       <c r="C20" s="2" t="s">
         <v>14</v>
       </c>
@@ -697,7 +690,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="6"/>
       <c r="C21" s="3" t="s">
         <v>4</v>
       </c>
@@ -706,7 +699,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="6"/>
       <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
@@ -718,7 +711,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="6"/>
       <c r="C23" s="3" t="s">
         <v>33</v>
       </c>
@@ -730,28 +723,28 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="C24" s="5" t="s">
+      <c r="A24" s="6"/>
+      <c r="C24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="6"/>
       <c r="C25" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="6"/>
       <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
@@ -759,10 +752,10 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="6"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C31" s="2" t="s">

</xml_diff>